<commit_message>
fix errors, redesigned functionality
</commit_message>
<xml_diff>
--- a/List of hours.xlsx
+++ b/List of hours.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\work-list\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud\Python\Michal\work-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="30">
   <si>
     <t>WYKAZ PRZEPRACOWANYCH GODZIN W MIESIĄCU</t>
   </si>
@@ -59,9 +59,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>UR</t>
-  </si>
-  <si>
     <t>Imię1 Nazwisko1</t>
   </si>
   <si>
@@ -86,10 +83,43 @@
     <t>ImięKierownika NazwiskoKierownika</t>
   </si>
   <si>
-    <t>Jan Kowalski</t>
-  </si>
-  <si>
-    <t>ERKO</t>
+    <t>U</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>UU</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t>SU</t>
+  </si>
+  <si>
+    <t>some additional remark made</t>
+  </si>
+  <si>
+    <t>Zbyszek Zbyszek</t>
+  </si>
+  <si>
+    <t>TeS-T_T</t>
+  </si>
+  <si>
+    <t>worked good</t>
+  </si>
+  <si>
+    <t>different coment</t>
+  </si>
+  <si>
+    <t>FirmX</t>
+  </si>
+  <si>
+    <t>John Snow</t>
   </si>
 </sst>
 </file>
@@ -639,7 +669,7 @@
   <dimension ref="A1:AH38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+      <selection activeCell="AI10" sqref="AI10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -734,7 +764,7 @@
       </c>
       <c r="C3" s="22"/>
       <c r="D3" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3" s="19"/>
@@ -760,7 +790,7 @@
       <c r="X3" s="22"/>
       <c r="Y3" s="22"/>
       <c r="Z3" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AA3" s="19"/>
       <c r="AB3" s="19"/>
@@ -882,10 +912,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>8</v>
@@ -978,7 +1008,7 @@
         <v>10</v>
       </c>
       <c r="AH6" s="7">
-        <f t="shared" ref="AH6:AH10" si="0">SUM(D6:AG6)</f>
+        <f t="shared" ref="AH6:AH11" si="0">SUM(D6:AG6)</f>
         <v>192</v>
       </c>
     </row>
@@ -987,10 +1017,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>8</v>
@@ -1092,10 +1122,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>8</v>
@@ -1197,20 +1227,18 @@
         <v>4</v>
       </c>
       <c r="B9" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="16">
+        <v>10</v>
+      </c>
+      <c r="E9" s="16"/>
+      <c r="F9" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>8</v>
-      </c>
       <c r="G9" s="14" t="s">
         <v>8</v>
       </c>
@@ -1218,7 +1246,7 @@
         <v>8</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="J9" s="16" t="s">
         <v>8</v>
@@ -1226,11 +1254,9 @@
       <c r="K9" s="16">
         <v>9</v>
       </c>
-      <c r="L9" s="16">
-        <v>10</v>
-      </c>
-      <c r="M9" s="17">
-        <v>8</v>
+      <c r="L9" s="16"/>
+      <c r="M9" s="17" t="s">
+        <v>27</v>
       </c>
       <c r="N9" s="14" t="s">
         <v>8</v>
@@ -1241,14 +1267,14 @@
       <c r="P9" s="16">
         <v>7</v>
       </c>
-      <c r="Q9" s="16">
-        <v>7</v>
+      <c r="Q9" s="16" t="s">
+        <v>19</v>
       </c>
       <c r="R9" s="16">
         <v>7</v>
       </c>
-      <c r="S9" s="16">
-        <v>10</v>
+      <c r="S9" s="16" t="s">
+        <v>20</v>
       </c>
       <c r="T9" s="17">
         <v>8</v>
@@ -1259,14 +1285,14 @@
       <c r="V9" s="16">
         <v>10</v>
       </c>
-      <c r="W9" s="16">
-        <v>8</v>
+      <c r="W9" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="X9" s="16">
         <v>10</v>
       </c>
       <c r="Y9" s="16">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="Z9" s="16">
         <v>10</v>
@@ -1277,24 +1303,24 @@
       <c r="AB9" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="AC9" s="16">
-        <v>10</v>
+      <c r="AC9" s="16" t="s">
+        <v>22</v>
       </c>
       <c r="AD9" s="16">
         <v>9</v>
       </c>
-      <c r="AE9" s="16">
-        <v>10</v>
+      <c r="AE9" s="16" t="s">
+        <v>23</v>
       </c>
       <c r="AF9" s="16">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AG9" s="16">
         <v>10</v>
       </c>
       <c r="AH9" s="7">
         <f t="shared" si="0"/>
-        <v>177</v>
+        <v>125.5</v>
       </c>
     </row>
     <row r="10" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1302,16 +1328,16 @@
         <v>5</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>8</v>
@@ -1323,10 +1349,10 @@
         <v>8</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="K10" s="16">
         <v>9</v>
@@ -1364,9 +1390,7 @@
       <c r="V10" s="16">
         <v>10</v>
       </c>
-      <c r="W10" s="16">
-        <v>10</v>
-      </c>
+      <c r="W10" s="16"/>
       <c r="X10" s="16">
         <v>10</v>
       </c>
@@ -1382,9 +1406,7 @@
       <c r="AB10" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="AC10" s="16">
-        <v>10</v>
-      </c>
+      <c r="AC10" s="16"/>
       <c r="AD10" s="16">
         <v>10</v>
       </c>
@@ -1399,15 +1421,118 @@
       </c>
       <c r="AH10" s="7">
         <f t="shared" si="0"/>
-        <v>192</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AF11" s="6"/>
-      <c r="AG11" s="6"/>
+      <c r="A11" s="7">
+        <v>6</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" s="16">
+        <v>9</v>
+      </c>
+      <c r="L11" s="16">
+        <v>10</v>
+      </c>
+      <c r="M11" s="17">
+        <v>8</v>
+      </c>
+      <c r="N11" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="O11" s="16">
+        <v>10</v>
+      </c>
+      <c r="P11" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q11" s="16">
+        <v>10</v>
+      </c>
+      <c r="R11" s="16">
+        <v>10</v>
+      </c>
+      <c r="S11" s="16">
+        <v>10</v>
+      </c>
+      <c r="T11" s="17">
+        <v>8</v>
+      </c>
+      <c r="U11" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="V11" s="16">
+        <v>10</v>
+      </c>
+      <c r="W11" s="16">
+        <v>10</v>
+      </c>
+      <c r="X11" s="16">
+        <v>10</v>
+      </c>
+      <c r="Y11" s="16">
+        <v>10</v>
+      </c>
+      <c r="Z11" s="16">
+        <v>10</v>
+      </c>
+      <c r="AA11" s="17">
+        <v>7</v>
+      </c>
+      <c r="AB11" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC11" s="16">
+        <v>10</v>
+      </c>
+      <c r="AD11" s="16">
+        <v>10</v>
+      </c>
+      <c r="AE11" s="16">
+        <v>10</v>
+      </c>
+      <c r="AF11" s="16">
+        <v>10</v>
+      </c>
+      <c r="AG11" s="16">
+        <v>10</v>
+      </c>
       <c r="AH11" s="7">
-        <f>SUM(AH6:AH10)</f>
-        <v>945</v>
+        <f t="shared" si="0"/>
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH12" s="7">
+        <f>SUM(AH7:AH11)</f>
+        <v>863.5</v>
       </c>
     </row>
     <row r="13" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>